<commit_message>
update tasks for 2sem
</commit_message>
<xml_diff>
--- a/Tasks_2_sem/Tasks_2.xlsx
+++ b/Tasks_2_sem/Tasks_2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Проги\Practice\Tasks_2_sem\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manan\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0F277AD-FFA3-4AC5-9B73-0CC50E6CA643}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED80E57-A934-4AA4-A3AC-10341F92FEB6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
-  <si>
-    <t>Начальное условие задачи</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="47">
   <si>
     <t>Отредактированное условие</t>
   </si>
@@ -39,38 +36,263 @@
     <t>Теги</t>
   </si>
   <si>
-    <t>Циклически сдвиньте элементы списка вправо (A[0] переходит на место A[1], A[1] на место A[2], ..., последний элемент переходит на место A[0]).</t>
-  </si>
-  <si>
-    <t>Через командную строку подается файл input.txt, в котором записан текст (на английском). Составить программу, которая сделает словарь из всех имеющихся слов и выведет 10 самых популярных слов.</t>
-  </si>
-  <si>
-    <t>Даны два отсортированных вектора. Написать функцию, которая объединяет их в один отсортированный вектор. Реализовать за O(n)</t>
-  </si>
-  <si>
-    <t>Даны два отсортированных по убываю  стека. Написать функцию, которая объединяет стеки в один с порядком по возрастанию.</t>
-  </si>
-  <si>
-    <t>Дана последовательность целых чисел, заканчивающаяся числом 0. Выведите эту последовательность в обратном порядке.
-При решении этой задачи нельзя пользоваться массивами и прочими динамическими структурами данных. Рекурсия вам поможет.</t>
-  </si>
-  <si>
-    <t>Напишите программу, реализующую игру "Угадай число". Компьютер загадывает число от 0 до 999 (используйте генерацию случайных чисел). На каждом шаге пользователь делает предположение, а компьютер сообщает, является ли это число больше, меньше или равно загаданному. Когда пользователь отгадывает задуманное число, игра заканчивается.</t>
-  </si>
-  <si>
-    <t>т</t>
-  </si>
-  <si>
-    <t>Напишите программу, которая объединяет два упорядоченных по возрастанию массива в один (тоже упорядоченный) массив.</t>
-  </si>
-  <si>
-    <t>Напишите программу, которая содержит текущую информацию о 10 заявках на авиабилеты. Каждая заявка имеет: пункт назначения, номер рейса, ФИО пассажира, желаемую дату вылета. Программа должна обеспечивать: хранение всех заявок в виде списка, добавление и удаление заявок, вывод всех заявок.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Напишите программу учета оценок студентов. Для этого создайте текстовый файл с именем input.txt, содержащий список из 10 студентов и их оценки по 3 предметам: математика, физика и информатика. Содержимое файла: в первой строке находится общее число студентов, в каждой следующей находится ФИО студента и три целых числа(оценки) (данные в строке отделяются пробелами). Создайте класс, с помощью которого вы будете считывать данные из файла. На экран выведите ФИО студентов с оценкаи в порядке убывания их среднего балла. </t>
-  </si>
-  <si>
-    <t>Создайте класс с именем Student, содержащую слудующие поля: Name, Year, Rating (успеваемость, массив из пяти элементов). Функции  класса: ввод данных в массив Rating, вывод в консоль записи, вывод среднего балла</t>
+    <t>Напишите функцию, которая циклически сдвигает элементы односвязного списка вправо
+(A[0] переходит на место A[1],  A[1] на место A[2], ..., последний элемент переходит на место A[0])
+Сигнатура: std::list&lt;int&gt; cyclicShift(std::list&lt;int&gt; input);</t>
+  </si>
+  <si>
+    <t>C++, сложность E, семестр 2, список</t>
+  </si>
+  <si>
+    <t>input: 1 2 3 4 5 6 7
+output: 7 1 2 3 4 5 6</t>
+  </si>
+  <si>
+    <t>C++, сложность E, семестр 2, словари, работа с файлами</t>
+  </si>
+  <si>
+    <t>В функцию подается название файла input.txt, в котором записан текст на английском.
+Реализовать функцию, которая сделает словарь из всех имеющихся слов и отсортирует его по популярности.
+Сигнатура: std::map&lt;std::string, int&gt; popularWord(std::string file);</t>
+  </si>
+  <si>
+    <t>input.txt:
+apple
+my apple,
+my red apple
+output:
+apple 3
+my 2
+red 1</t>
+  </si>
+  <si>
+    <t>C++, сложность D, семестр 2, вектор, сортировка</t>
+  </si>
+  <si>
+    <t>Даны два отсортированных вектора целых чисел. 
+Написать функцию, которая объединяет их в один отсортированный вектор. Реализовать за O(n).
+Сигнатура: std::vector&lt;int&gt; sumVect(std::vector&lt;int&gt; vec_f, std::vector&lt;int&gt; vec_s);</t>
+  </si>
+  <si>
+    <t>input: 
+-5 -1 4 6
+-6 -3 0 1 5 8
+output:
+-6 -5 -3 -1 0 1 4 5 6 8</t>
+  </si>
+  <si>
+    <t>Даны два отсортированных по убыванию стека. Написать функцию,
+которая объединяет стеки в один с порядком по возрастанию.
+Сигнатура: std::stack&lt;int&gt; sorted(std::stack&lt;int&gt; first, std::stack&lt;int&gt; second);</t>
+  </si>
+  <si>
+    <t>C++, сложность D, семестр 2, стек, сортировка</t>
+  </si>
+  <si>
+    <t>input: 
+8, 4, 2, -5
+5, 2, -1
+output:
+-5, -1, 2, 2, 4, 5, 8</t>
+  </si>
+  <si>
+    <t>Напишите функцию, которая разворачивает вектор целых чисел.
+Сигнатура: std::vector&lt;int&gt; reverseVec(std::vector&lt;int&gt; vec);</t>
+  </si>
+  <si>
+    <t>C++, сложность E, семестр 2, вектор</t>
+  </si>
+  <si>
+    <t>input: 1 2 3 4 5
+output: 5 4 3 2 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> C++, сложность D, семестр 2, массив, сортировка</t>
+  </si>
+  <si>
+    <t>Напишите программу, которая объединяет два упорядоченных по возрастанию
+массива в один (тоже упорядоченный) массив.
+Сигнатура: int* sortedArray(int* one, int* two);</t>
+  </si>
+  <si>
+    <t>input:
+-2 1 4
+-3 -2 0
+output:
+-3 -2 -2 1 0 4</t>
+  </si>
+  <si>
+    <t>На вход подается отсортированный по возрастанию вектор целых чисел. 
+Напишите функцию, которая возращает отсортированный по возрастанию вектор квадратов значений данного вектора.</t>
+  </si>
+  <si>
+    <t>input:
+-4, -1, 0, 1, 2, 4, 6
+output:
+0, 1, 1, 2, 16, 16, 36</t>
+  </si>
+  <si>
+    <t>Напишите программу, реализующую игру "Угадай число".
+Компьютер загадывает число от 0 до 999 (используйте генерацию случайных чисел). 
+На каждом шаге пользователь делает предположение, а компьютер сообщает, 
+является ли это число больше, меньше или равно загаданному. 
+Когда пользователь отгадывает задуманное число, игра заканчивается.</t>
+  </si>
+  <si>
+    <t>C++, сложность D, семестр 2, генерация чисел, циклы</t>
+  </si>
+  <si>
+    <t>Напишите программу, которая содержит текущую информацию о 10 заявках на авиабилеты. 
+Каждая заявка имеет: 
+* пункт назначения
+* номер рейса 
+* ФИО пассажира 
+* желаемую дату вылета.
+Программа должна обеспечивать: 
+1. хранение всех заявок в виде списка
+2. добавление заявок
+3. удаление заявок
+4. вывод всех заявок.</t>
+  </si>
+  <si>
+    <t>C++, сложность С, семестр 2, ООП</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Напишите программу учета оценок студентов. 
+Для этого создайте текстовый файл с именем input.txt, содержащий список 
+из 10 студентов и их оценки по 3 предметам: математика, физика и информатика. 
+Содержимое файла: в первой строке находится общее число студентов, 
+в каждой следующей находится ФИО студента и три целых числа(оценки). Данные в строке отделяются пробелами. 
+Создайте класс, с помощью которого вы будете считывать данные из файла.
+На экран выведите ФИО студентов с оценкаи в порядке убывания их среднего балла. </t>
+  </si>
+  <si>
+    <t>C++, сложность С, семестр 2, ООП, работа с файласм</t>
+  </si>
+  <si>
+    <t>Создайте класс с именем Student, содержащую слудующие поля: 
+Name, 
+Year, 
+Rating (успеваемость, массив из пяти элементов).
+Функции  класса: 
+* ввод данных в массив Rating, 
+* вывод в консоль записи, 
+* вывод среднего балла</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> C++, сложность С, семестр 2, ООП</t>
+  </si>
+  <si>
+    <t>Создайте класс Деньги для работы с денежными суммами. 
+Число должно быть представлено двумя полями: 
+типа long для рублей и типа unsigned char - для копеек. 
+Дробная часть (копейки) при выводе на экран должна быть отделена от целой части запятой. 
+Реализовать:
+1. сложение
+2. вычитание
+3. деление сумм
+4. деление суммы на дробное число, 
+5. умножение на дробное число
+6. операции сравнения. 
+В функции main проверить эти методы.</t>
+  </si>
+  <si>
+    <t>Разработать три класса, которые следует связать между собой, используя наследование:
+* класс Product, который имеет три элемент-данных — имя, цена и вес товара (базовый класс для всех классов);
+* класс Buy, содержащий данные о количестве покупаемого товара в штуках, 
+  о цене за весь купленный товар и о весе товара (производный класс для класса 
+  Product и базовый класс для класса Check);
+* класс Check, не содержащий никаких элемент-данных. 
+  Данный класс должен выводить на экран информацию о товаре и о покупке ( производный класс для класса Buy);
+Для взаимодействия с данными классов разработать set- и get—методы. 
+Все элемент-данные классов объявлять как private.</t>
+  </si>
+  <si>
+    <t>Дана последовательность целых чисел, заканчивающаяся числом 0. 
+Выведите эту последовательность в обратном порядке.
+При решении этой задачи нельзя пользоваться массивами и прочими динамическими
+структурами данных. Рекурсия вам поможет.</t>
+  </si>
+  <si>
+    <t>C++, сложность E, семестр 2</t>
+  </si>
+  <si>
+    <t>Реализовать класс матрицы целых чисел. Размерность матриц не ограничена. Класс должен:
+* считывать элементы матрицы из файла формата csv;
+* реализовывать конструкторы копирования и перемещения (если необходимо);
+* реализовывать операторы копирующего и перемещающего присваивания (если необходимо);
+* реализовывать операторы сложения, вычитания, умножения матриц;
+* обрабатывать ошибки с использованием исключений</t>
+  </si>
+  <si>
+    <t>C++, сложность B, семестр 2, массивы, ООП</t>
+  </si>
+  <si>
+    <t>Напишите программу, которая будет выводить календарь на месяц и год, который вводит пользователь.
+P.s. отсчет вести от 01.01.1919 (среда)</t>
+  </si>
+  <si>
+    <t>input: 5 2022
+output: 
+Mo Tu We Th Fr Sa Su
+                                        1
+  2    3    4    5    6    7   8
+  9  10  11  12  13 14 15
+16  17 18  19  20  21 22
+23  24 25  26  27  28 29
+30  31</t>
+  </si>
+  <si>
+    <t>Пользователь вводит число N. Написать программу, которая выводит спиральный массив.
+Спиральный   массив   представляет собой квадратное расположение первых   N^2   натуральных чисел, где
+числа последовательно увеличиваются по мере того, как вы идете по краям массива по спирали внутрь.</t>
+  </si>
+  <si>
+    <t>input:
+5
+output:
+0 1 2 3 4
+15 16 17 18 5
+14 23 24 19 6
+13 22 21 20 7
+12 11 10 9 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> C++, сложность E, семестр 2</t>
+  </si>
+  <si>
+    <t>Игра   «Свинья»   — это многопользовательская игра, в которой используется один шестигранный кубик. 
+Цель игры —   набрать 100   и более очков. Игра ведется по очереди. В свой ход у этого человека есть выбор:
+1. Бросание костей : когда к их счету за этот ход добавляется результат от двух до шести, и ход игрока продолжается, 
+поскольку игроку снова предоставляется тот же выбор; или бросок   1   теряет общее количество очков игрока   за этот ход,
+и его ход заканчивается передачей игры следующему игроку.
+2. Удерживание : счет игрока за этот раунд добавляется к его общему количеству и становится безопасным от эффектов
+выбрасывания   1   (единицы). Ход игрока заканчивается передачей хода следующему игроку.
+Создайте программу для подсчета очков и имитации бросков костей в игре для двух человек.</t>
+  </si>
+  <si>
+    <t>C++, сложность E, семестр 2, случайная генерация</t>
+  </si>
+  <si>
+    <t>Число вампира — это натуральное десятичное число с четным количеством цифр, которое можно разложить на два целых числа.
+Эти два числа называются клыками и должны обладать следующими свойствами:
+ * каждый из них содержит половину десятичных цифр исходного числа
+ * вместе они состоят из тех же десятичных цифр, что и исходное число
+ * самое большее одно из них имеет конечный ноль
+Выведите первые N чисел вампиров и их клыки
+Пример номера вампира и его клыков:   1260 : (21, 60)</t>
+  </si>
+  <si>
+    <t>Отсортируйте массив (или список) элементов, используя алгоритм сортировки выбором.
+Это работает следующим образом:
+Сначала найдите в массиве наименьший элемент и замените его на элемент в первой позиции, затем найдите второй наименьший 
+элемент и замените его на элемент во второй позиции, и так далее, пока весь массив не будет отсортирован.
+Его асимптотическая сложность составляет   O (n 2 )   , что делает его неэффективным на больших массивах.
+Его основная цель - когда запись данных очень дорогая (медленная) по сравнению с чтением, например. запись во флэш-память или EEPROM.
+Никакой другой алгоритм сортировки не имеет меньшего количества перемещений данных.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> C++, сложность E, семестр 2, массивы, сортировка</t>
   </si>
 </sst>
 </file>
@@ -430,21 +652,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="54.26953125" customWidth="1"/>
-    <col min="2" max="2" width="58.26953125" customWidth="1"/>
-    <col min="3" max="3" width="48.26953125" customWidth="1"/>
-    <col min="4" max="4" width="29" customWidth="1"/>
+    <col min="1" max="1" width="58.28515625" customWidth="1"/>
+    <col min="2" max="2" width="48.28515625" customWidth="1"/>
+    <col min="3" max="3" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -454,235 +675,274 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="100" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:4" ht="100" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="1"/>
+    </row>
+    <row r="3" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:4" ht="100" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="1"/>
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" ht="100" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="1"/>
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" ht="100" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:4" ht="100" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="1"/>
+        <v>17</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="B7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:4" ht="100" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:4" ht="100" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:4" ht="132.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:4" ht="100" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="1:4" ht="100" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="1"/>
+    </row>
+    <row r="9" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="180" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="195" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="1:4" ht="100" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="1"/>
+      <c r="C12" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="195" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:4" ht="100" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="1"/>
+      <c r="C13" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="225" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="1:4" ht="100" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="1"/>
+      <c r="C14" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="1:4" ht="100" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="1"/>
+      <c r="C15" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="1:4" ht="100" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="1:4" ht="100" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="1:4" ht="100" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="1"/>
+      <c r="C16" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="255" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="1:4" ht="100" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="1"/>
+      <c r="C19" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="180" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="1:4" ht="100" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="1"/>
+      <c r="C20" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="225" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="1:4" ht="100" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C21" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="1:4" ht="100" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="23" spans="1:3" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="1:4" ht="100" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="24" spans="1:3" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="1:4" ht="100" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="25" spans="1:3" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="1:4" ht="100" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="26" spans="1:3" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="1:4" ht="100" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="27" spans="1:3" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-    </row>
-    <row r="28" spans="1:4" ht="100" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="28" spans="1:3" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="1:4" ht="100" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="29" spans="1:3" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="1:4" ht="100" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="30" spans="1:3" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="1:4" ht="100" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="31" spans="1:3" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="1:4" ht="100" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="32" spans="1:3" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="1:4" ht="100" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="33" spans="1:3" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-    </row>
-    <row r="34" spans="1:4" ht="100" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="34" spans="1:3" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-    </row>
-    <row r="35" spans="1:4" ht="100" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="35" spans="1:3" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>